<commit_message>
Committing ULP regression test case changes
Vinay - 06/01/2023
</commit_message>
<xml_diff>
--- a/Data Files/Functional Regression/MultiStateAddress.xlsx
+++ b/Data Files/Functional Regression/MultiStateAddress.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motuvin\Katalon Studio\HMIC-Portal\Data Files\Functional Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68305E28-92F9-44EE-BCBF-5F7933D05D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D51D6A-2452-4A25-9E9B-14815E504DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1010,10 +1010,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Vinay - ULP New Rate Changes - 06/07/2023
</commit_message>
<xml_diff>
--- a/Data Files/Functional Regression/MultiStateAddress.xlsx
+++ b/Data Files/Functional Regression/MultiStateAddress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motuvin\Katalon Studio\HMIC-Portal\Data Files\Functional Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D51D6A-2452-4A25-9E9B-14815E504DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEBFB85-4292-4BEC-85F4-B312D4656CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IA" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,27 @@
     <sheet name="IN" sheetId="3" r:id="rId3"/>
     <sheet name="IL" sheetId="4" r:id="rId4"/>
     <sheet name="WI" sheetId="5" r:id="rId5"/>
+    <sheet name="OH" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>Address</t>
   </si>
@@ -45,6 +59,9 @@
   </si>
   <si>
     <t>955 N Mutual Way</t>
+  </si>
+  <si>
+    <t>3900 Morse Rd</t>
   </si>
 </sst>
 </file>
@@ -1009,7 +1026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4139A73B-3DF6-4EA5-B19A-28973C63F24F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -1037,4 +1054,38 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F211B6C-BDBB-4C0F-81E8-17420D79AB33}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>43219</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Vinay - ULP Changes - 0628
</commit_message>
<xml_diff>
--- a/Data Files/Functional Regression/MultiStateAddress.xlsx
+++ b/Data Files/Functional Regression/MultiStateAddress.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motuvin\Katalon Studio\HMIC-Portal\Data Files\Functional Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEBFB85-4292-4BEC-85F4-B312D4656CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69681C79-D976-4EC5-9313-3752E507948A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>Address</t>
   </si>
@@ -62,6 +62,27 @@
   </si>
   <si>
     <t>3900 Morse Rd</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>OH</t>
   </si>
 </sst>
 </file>
@@ -902,26 +923,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>50010</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -931,28 +960,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172CC227-35F3-41BD-A509-C587357BB7BA}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
         <v>49058</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -962,28 +997,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56AC5FF9-748E-44BF-B24B-405D1DE15FDA}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
         <v>46268</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -993,28 +1034,34 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B64FAEB8-B539-414E-B4DB-348FCE69A5C6}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
         <v>61604</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1024,10 +1071,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4139A73B-3DF6-4EA5-B19A-28973C63F24F}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1035,20 +1082,26 @@
     <col min="1" max="1" width="16.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
         <v>54956</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1058,10 +1111,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F211B6C-BDBB-4C0F-81E8-17420D79AB33}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1069,20 +1122,26 @@
     <col min="1" max="1" width="13.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2">
         <v>43219</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>